<commit_message>
Updated BOM with Digikey part numbers
</commit_message>
<xml_diff>
--- a/Mainbord BOM.xlsx
+++ b/Mainbord BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="6140" windowWidth="24720" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="0" windowWidth="24020" windowHeight="18880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="161">
   <si>
     <t>Qty</t>
   </si>
@@ -326,9 +326,6 @@
     <t>MIC803</t>
   </si>
   <si>
-    <t>MIC803-31D3VM3TR</t>
-  </si>
-  <si>
     <t>SOT95P232X110-3N</t>
   </si>
   <si>
@@ -477,13 +474,83 @@
   </si>
   <si>
     <t>535-9808-1-ND</t>
+  </si>
+  <si>
+    <t>587-1287-1-ND</t>
+  </si>
+  <si>
+    <t>399-1158-1-ND</t>
+  </si>
+  <si>
+    <t>399-1151-1-ND</t>
+  </si>
+  <si>
+    <t>399-7158-1-ND</t>
+  </si>
+  <si>
+    <t>399-5620-1-ND</t>
+  </si>
+  <si>
+    <t>408-1556-1-ND</t>
+  </si>
+  <si>
+    <t>311-.75SCT-ND</t>
+  </si>
+  <si>
+    <t>1276-6000-1-ND</t>
+  </si>
+  <si>
+    <t>311-10KARCT-ND</t>
+  </si>
+  <si>
+    <t>311-33.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t>311-4.70KCRCT-ND</t>
+  </si>
+  <si>
+    <t>RHM470CHCT-ND</t>
+  </si>
+  <si>
+    <t>311-68.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t>RHC2512FT7R50CT-ND</t>
+  </si>
+  <si>
+    <t>ZXMP2120FFCT-ND</t>
+  </si>
+  <si>
+    <t>MIC803-31D2VM3TR</t>
+  </si>
+  <si>
+    <t>576-3814-1-ND</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Newark </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>69W6470</t>
+    </r>
+  </si>
+  <si>
+    <t>342-1082-1-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -506,6 +573,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -530,9 +610,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -873,7 +954,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -914,7 +995,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -928,21 +1009,21 @@
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -951,13 +1032,16 @@
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -971,13 +1055,16 @@
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -991,7 +1078,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
         <v>27</v>
@@ -1000,7 +1087,7 @@
         <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1014,7 +1101,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
@@ -1023,7 +1110,7 @@
         <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1037,7 +1124,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
@@ -1045,6 +1132,9 @@
       <c r="F7" t="s">
         <v>9</v>
       </c>
+      <c r="G7" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8">
@@ -1057,13 +1147,16 @@
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" t="s">
         <v>48</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1077,7 +1170,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E9" t="s">
         <v>44</v>
@@ -1086,7 +1179,7 @@
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1107,6 +1200,9 @@
       </c>
       <c r="F10" t="s">
         <v>9</v>
+      </c>
+      <c r="G10" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1129,7 +1225,7 @@
         <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1137,22 +1233,22 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" t="s">
         <v>130</v>
-      </c>
-      <c r="C12" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" t="s">
-        <v>111</v>
-      </c>
-      <c r="F12" t="s">
-        <v>114</v>
-      </c>
-      <c r="G12" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1160,22 +1256,22 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1189,7 +1285,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -1197,6 +1293,9 @@
       <c r="F14" t="s">
         <v>8</v>
       </c>
+      <c r="G14" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
@@ -1209,7 +1308,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
@@ -1217,6 +1316,9 @@
       <c r="F15" t="s">
         <v>8</v>
       </c>
+      <c r="G15" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
@@ -1236,6 +1338,9 @@
       </c>
       <c r="F16" t="s">
         <v>8</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1249,7 +1354,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E17" t="s">
         <v>18</v>
@@ -1258,7 +1363,7 @@
         <v>8</v>
       </c>
       <c r="G17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1272,7 +1377,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E18" t="s">
         <v>22</v>
@@ -1280,6 +1385,9 @@
       <c r="F18" t="s">
         <v>8</v>
       </c>
+      <c r="G18" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19">
@@ -1292,16 +1400,16 @@
         <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
       </c>
       <c r="G19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1315,7 +1423,7 @@
         <v>8</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" t="s">
         <v>29</v>
@@ -1324,7 +1432,7 @@
         <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1338,7 +1446,7 @@
         <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E21" t="s">
         <v>37</v>
@@ -1347,7 +1455,7 @@
         <v>8</v>
       </c>
       <c r="G21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1361,13 +1469,16 @@
         <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E22" t="s">
         <v>39</v>
       </c>
       <c r="F22" t="s">
         <v>8</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1375,13 +1486,13 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C23" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E23" t="s">
         <v>40</v>
@@ -1390,7 +1501,7 @@
         <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1404,7 +1515,7 @@
         <v>8</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E24" t="s">
         <v>42</v>
@@ -1412,6 +1523,9 @@
       <c r="F24" t="s">
         <v>8</v>
       </c>
+      <c r="G24" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25">
@@ -1424,7 +1538,7 @@
         <v>8</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E25" t="s">
         <v>46</v>
@@ -1432,6 +1546,9 @@
       <c r="F25" t="s">
         <v>8</v>
       </c>
+      <c r="G25" s="2" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
@@ -1444,7 +1561,7 @@
         <v>8</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E26" t="s">
         <v>52</v>
@@ -1453,7 +1570,7 @@
         <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1467,13 +1584,16 @@
         <v>8</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E27" t="s">
         <v>54</v>
       </c>
       <c r="F27" t="s">
         <v>8</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1495,6 +1615,9 @@
       <c r="F28" t="s">
         <v>8</v>
       </c>
+      <c r="G28" s="2" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29">
@@ -1504,7 +1627,7 @@
         <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>59</v>
@@ -1516,7 +1639,7 @@
         <v>61</v>
       </c>
       <c r="G29" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1524,19 +1647,22 @@
         <v>2</v>
       </c>
       <c r="B30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" t="s">
         <v>97</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>98</v>
       </c>
-      <c r="F30" t="s">
-        <v>99</v>
+      <c r="G30" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1544,19 +1670,19 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C31" t="s">
-        <v>100</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" t="s">
         <v>101</v>
       </c>
-      <c r="E31" t="s">
-        <v>102</v>
-      </c>
       <c r="G31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1564,19 +1690,19 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" t="s">
         <v>106</v>
       </c>
-      <c r="C32" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" t="s">
-        <v>107</v>
-      </c>
       <c r="G32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1596,7 +1722,7 @@
         <v>72</v>
       </c>
       <c r="G33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1607,16 +1733,19 @@
         <v>91</v>
       </c>
       <c r="C34" t="s">
+        <v>157</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" t="s">
         <v>93</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>94</v>
       </c>
-      <c r="F34" t="s">
-        <v>95</v>
+      <c r="G34" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1635,6 +1764,9 @@
       <c r="E35" t="s">
         <v>57</v>
       </c>
+      <c r="G35" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36">
@@ -1655,6 +1787,9 @@
       <c r="F36" t="s">
         <v>79</v>
       </c>
+      <c r="G36" s="2" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37">
@@ -1693,7 +1828,7 @@
         <v>86</v>
       </c>
       <c r="G38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1701,19 +1836,19 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E39" t="s">
         <v>103</v>
       </c>
-      <c r="C39" t="s">
-        <v>103</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>104</v>
-      </c>
-      <c r="F39" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1721,19 +1856,19 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40" t="s">
         <v>109</v>
       </c>
-      <c r="C40" t="s">
-        <v>109</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E40" t="s">
-        <v>110</v>
-      </c>
       <c r="F40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1753,7 +1888,7 @@
         <v>69</v>
       </c>
       <c r="G41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:7">

</xml_diff>

<commit_message>
Beginning of new solar panel layout
Changing to pairs of TASC cells to accommodate irregularities in
dimensions
</commit_message>
<xml_diff>
--- a/Mainbord BOM.xlsx
+++ b/Mainbord BOM.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="1040" windowWidth="24020" windowHeight="18880" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24820" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -994,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>